<commit_message>
#4 additional evaluation files
</commit_message>
<xml_diff>
--- a/bernard/experiment/results/results_complete/tap_res_quant_0.95.xlsx
+++ b/bernard/experiment/results/results_complete/tap_res_quant_0.95.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="reimb" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="student" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="real" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delay1.0" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delay0.5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,10 +440,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ftap_1_wu_50</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_50</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>ftap_1_wu_0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>bern_wu_0</t>
         </is>
@@ -458,6 +471,12 @@
       <c r="C2" t="n">
         <v>50</v>
       </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -471,6 +490,12 @@
       <c r="C3" t="n">
         <v>5</v>
       </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -479,9 +504,15 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>755</v>
+        <v>731</v>
       </c>
       <c r="C4" t="n">
+        <v>42</v>
+      </c>
+      <c r="D4" t="n">
+        <v>752</v>
+      </c>
+      <c r="E4" t="n">
         <v>45</v>
       </c>
     </row>
@@ -497,6 +528,12 @@
       <c r="C5" t="n">
         <v>45</v>
       </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -505,9 +542,15 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1914</v>
+        <v>1888</v>
       </c>
       <c r="C6" t="n">
+        <v>2577</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1917</v>
+      </c>
+      <c r="E6" t="n">
         <v>2624</v>
       </c>
     </row>
@@ -518,9 +561,15 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06211180124223602</v>
+        <v>0.06402048655569782</v>
       </c>
       <c r="C7" t="n">
+        <v>0.1063829787234043</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.06234413965087282</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -536,6 +585,12 @@
       <c r="C8" t="n">
         <v>0.1</v>
       </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -544,9 +599,15 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2828774822030723</v>
+        <v>0.2791141657121038</v>
       </c>
       <c r="C9" t="n">
+        <v>0.01603665521191294</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2817534657174972</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.01686024728362683</v>
       </c>
     </row>
@@ -557,10 +618,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6464620353465055</v>
+        <v>0.6948370160141883</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6463423256225005</v>
+        <v>0.6947229302369489</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6947229302369489</v>
       </c>
     </row>
     <row r="11">
@@ -570,9 +637,15 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1169590643274854</v>
+        <v>0.1203369434416366</v>
       </c>
       <c r="C11" t="n">
+        <v>0.1030927835051546</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1173708920187793</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -583,9 +656,15 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.937888198757764</v>
+        <v>0.9158249158249158</v>
       </c>
       <c r="C12" t="n">
+        <v>0.5383227242031354</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.9376558603491272</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.570857007957476</v>
       </c>
     </row>
@@ -600,7 +679,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,10 +690,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ftap_1_wu_50</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_50</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>ftap_1_wu_0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>bern_wu_0</t>
         </is>
@@ -627,9 +716,15 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>49</v>
+      </c>
+      <c r="C2" t="n">
+        <v>49</v>
+      </c>
+      <c r="D2" t="n">
         <v>50</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>50</v>
       </c>
     </row>
@@ -640,10 +735,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -653,10 +754,16 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>409</v>
+      </c>
+      <c r="C4" t="n">
+        <v>36</v>
+      </c>
+      <c r="D4" t="n">
         <v>435</v>
       </c>
-      <c r="C4" t="n">
-        <v>41</v>
+      <c r="E4" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -666,10 +773,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="6">
@@ -679,10 +792,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1052</v>
+        <v>1031</v>
       </c>
       <c r="C6" t="n">
-        <v>1446</v>
+        <v>1404</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1054</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1449</v>
       </c>
     </row>
     <row r="7">
@@ -692,10 +811,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.09937888198757763</v>
+        <v>0.1069868995633188</v>
       </c>
       <c r="C7" t="n">
-        <v>0.18</v>
+        <v>0.2173913043478261</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1030927835051546</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
@@ -705,10 +830,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.18</v>
+        <v>0.2040816326530612</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
@@ -718,10 +849,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2925353059852051</v>
+        <v>0.2840277777777778</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02757229320780094</v>
+        <v>0.025</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2921423774345198</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.02686366689053056</v>
       </c>
     </row>
     <row r="10">
@@ -731,10 +868,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6464620353465055</v>
+        <v>0.6948370160141883</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6463423256225005</v>
+        <v>0.6947229302369489</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6947229302369489</v>
       </c>
     </row>
     <row r="11">
@@ -744,10 +887,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1801125703564728</v>
+        <v>0.1932938856015779</v>
       </c>
       <c r="C11" t="n">
-        <v>0.18</v>
+        <v>0.2105263157894737</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1869158878504673</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="12">
@@ -757,10 +906,766 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8967617594264092</v>
+        <v>0.864840118326525</v>
       </c>
       <c r="C12" t="n">
-        <v>0.583170245782498</v>
+        <v>0.5544983556807068</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.8969072164948454</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5808506411066303</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ftap_1_wu_50</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_50</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ftap_1_wu_0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>traces</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>21736</v>
+      </c>
+      <c r="C2" t="n">
+        <v>21736</v>
+      </c>
+      <c r="D2" t="n">
+        <v>21744</v>
+      </c>
+      <c r="E2" t="n">
+        <v>21744</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>tp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11310</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15860</v>
+      </c>
+      <c r="D3" t="n">
+        <v>11315</v>
+      </c>
+      <c r="E3" t="n">
+        <v>15868</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>fp</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3199</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5870</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3207</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>fn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10426</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5876</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10429</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>tn</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>75907</v>
+      </c>
+      <c r="C6" t="n">
+        <v>73236</v>
+      </c>
+      <c r="D6" t="n">
+        <v>75941</v>
+      </c>
+      <c r="E6" t="n">
+        <v>73272</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>prec</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.7795161623819699</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.7298665439484584</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.7791626497727586</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.7297645327446652</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>tpr_recall</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5203349282296651</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7296650717703349</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5203734363502576</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.7297645327446652</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>fpr</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0404394104113468</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.07420423229590675</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.040519027644413</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.07424066306160611</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.6947229302369489</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6947229302369489</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>fscore</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.6240860808387364</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.7297657939538948</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.6240004411845808</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.7297645327446652</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.3215360223044577</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.3141920161817572</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3225014550576006</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.3147220061256978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ftap_1_wu_50</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_50</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ftap_1_wu_0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>traces</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>984</v>
+      </c>
+      <c r="C2" t="n">
+        <v>984</v>
+      </c>
+      <c r="D2" t="n">
+        <v>990</v>
+      </c>
+      <c r="E2" t="n">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>tp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>450</v>
+      </c>
+      <c r="C3" t="n">
+        <v>360</v>
+      </c>
+      <c r="D3" t="n">
+        <v>452</v>
+      </c>
+      <c r="E3" t="n">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>fp</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>802</v>
+      </c>
+      <c r="C4" t="n">
+        <v>618</v>
+      </c>
+      <c r="D4" t="n">
+        <v>814</v>
+      </c>
+      <c r="E4" t="n">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>fn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>534</v>
+      </c>
+      <c r="C5" t="n">
+        <v>624</v>
+      </c>
+      <c r="D5" t="n">
+        <v>538</v>
+      </c>
+      <c r="E5" t="n">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>tn</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4183</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4367</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4215</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4401</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>prec</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.3594249201277955</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3680981595092024</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.3570300157977883</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3656565656565657</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>tpr_recall</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4573170731707317</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.3658536585365854</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4565656565656566</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.3656565656565657</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>fpr</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1608826479438315</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1239719157472417</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1618612050109366</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1248757208192484</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.6947229302369489</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6947229302369489</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>fscore</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.4025044722719142</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3669724770642201</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.4007092198581561</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3656565656565657</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5417865559203369</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5264836958640515</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5470963488447895</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5316622342277069</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ftap_1_wu_50</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_50</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ftap_1_wu_0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>bern_wu_0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>traces</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>984</v>
+      </c>
+      <c r="C2" t="n">
+        <v>984</v>
+      </c>
+      <c r="D2" t="n">
+        <v>990</v>
+      </c>
+      <c r="E2" t="n">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>tp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>305</v>
+      </c>
+      <c r="C3" t="n">
+        <v>258</v>
+      </c>
+      <c r="D3" t="n">
+        <v>307</v>
+      </c>
+      <c r="E3" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>fp</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>883</v>
+      </c>
+      <c r="C4" t="n">
+        <v>719</v>
+      </c>
+      <c r="D4" t="n">
+        <v>895</v>
+      </c>
+      <c r="E4" t="n">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>fn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>679</v>
+      </c>
+      <c r="C5" t="n">
+        <v>726</v>
+      </c>
+      <c r="D5" t="n">
+        <v>683</v>
+      </c>
+      <c r="E5" t="n">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>tn</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4102</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4266</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4134</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4299</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>prec</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.2567340067340068</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.2640736949846469</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2554076539101497</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.2626262626262627</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>tpr_recall</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.3099593495934959</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2621951219512195</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3101010101010101</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2626262626262627</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>fpr</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1771313941825476</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1442326980942829</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1779677868363492</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1451580831179161</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>auc</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.6947229302369489</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6948370160141883</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6947229302369489</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>fscore</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.2808471454880295</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.2631310555838857</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.2801094890510949</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2626262626262627</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5938351345570101</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5756722371549983</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.597496364849579</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5799345435327842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>